<commit_message>
g_feat: Add GraphBuilder service for transforming family data into Cytoscape elements using depth-based merging and positioning.
</commit_message>
<xml_diff>
--- a/복사본 가계도샘플.xlsx
+++ b/복사본 가계도샘플.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1731a6af20375572/E^0B_STUDIO/FamilyTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{064A6FDD-71F4-4F38-A283-6179F5664FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7DC597C-BC9B-4FE4-9A20-EA77C74A629B}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{064A6FDD-71F4-4F38-A283-6179F5664FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A850BC23-1679-4665-A926-13EC7AABFFB4}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2F259C8C-EF31-4814-8CFC-98BEC894FA59}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R9" sqref="R9"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -608,7 +608,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -676,7 +676,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
+      <selection pane="bottomLeft" sqref="A1:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -852,7 +852,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
g_feat: Introduce GraphBuilder service to transform family data into Cytoscape graph elements using a depth-based layout.
</commit_message>
<xml_diff>
--- a/복사본 가계도샘플.xlsx
+++ b/복사본 가계도샘플.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/1731a6af20375572/E^0B_STUDIO/FamilyTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="8_{064A6FDD-71F4-4F38-A283-6179F5664FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A850BC23-1679-4665-A926-13EC7AABFFB4}"/>
+  <xr:revisionPtr revIDLastSave="53" documentId="8_{064A6FDD-71F4-4F38-A283-6179F5664FEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{84B4E6BB-A8B9-4790-A73A-60DAAEC7CDD2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{2F259C8C-EF31-4814-8CFC-98BEC894FA59}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{2F259C8C-EF31-4814-8CFC-98BEC894FA59}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="35">
   <si>
     <t>이름</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -141,6 +141,42 @@
   </si>
   <si>
     <t>이채봉</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>큰고모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은고모</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>큰고모부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>작은고모부</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김춘식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김제식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>김간식</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍성우</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>홍성수</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -525,13 +561,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32429C7A-8D77-4FA6-A4F4-688493A68397}">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -662,6 +702,86 @@
       </c>
       <c r="C16" t="s">
         <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="C25" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -672,14 +792,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED98E317-5E38-4319-8EEB-791C2E14A5C3}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:B20"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -839,6 +962,118 @@
       </c>
       <c r="B20" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -851,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{82ADC434-4E7B-4E6F-81C9-C8DADD2EDA39}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>